<commit_message>
Added Row 6 to the excel
</commit_message>
<xml_diff>
--- a/5.xlsx
+++ b/5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lavinia.nastase\Documents\2021\Redo SA Training\BestPractices_Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/minal_gupta_uipath_com/Documents/Desktop/Training/Solution Architect/Training Material - TO be Shared/TO SHARE_2023/BestPractices_Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF55128-50E1-4CA4-9E65-55527B5607C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0CF55128-50E1-4CA4-9E65-55527B5607C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DF37980-6698-43F4-97B3-348EA58E05C2}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>No</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>VP</t>
+  </si>
+  <si>
+    <t>Minal</t>
+  </si>
+  <si>
+    <t>RPA Consultant</t>
   </si>
 </sst>
 </file>
@@ -381,18 +387,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -414,7 +420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -425,7 +431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -436,7 +442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -447,7 +453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -456,6 +462,17 @@
       </c>
       <c r="C6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -464,6 +481,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DB0EACA04781F346B2F5F63A17864137" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0075c12727a7ed827c4322e9554145ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5756a67b-a28b-4cf5-88e6-2b4468392c6e" xmlns:ns3="2ace790c-9bff-4836-93d2-c906c881a70a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f08f5f6833109816820f85ad85e3752f" ns2:_="" ns3:_="">
     <xsd:import namespace="5756a67b-a28b-4cf5-88e6-2b4468392c6e"/>
@@ -720,15 +746,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -748,13 +765,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B86CF1-6E85-4612-ADF7-5D48543D5046}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DE48AD1-55EB-41A4-AEE2-E77CC067AE09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DE48AD1-55EB-41A4-AEE2-E77CC067AE09}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39B86CF1-6E85-4612-ADF7-5D48543D5046}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5756a67b-a28b-4cf5-88e6-2b4468392c6e"/>
+    <ds:schemaRef ds:uri="2ace790c-9bff-4836-93d2-c906c881a70a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EB81F4-EE4E-4AD3-AF7D-07F4948F40BF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6EB81F4-EE4E-4AD3-AF7D-07F4948F40BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5756a67b-a28b-4cf5-88e6-2b4468392c6e"/>
+    <ds:schemaRef ds:uri="2ace790c-9bff-4836-93d2-c906c881a70a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>